<commit_message>
Tidied up ADC sampling code. Made loading indicator nicer.
</commit_message>
<xml_diff>
--- a/docs/adc-calibration.xlsx
+++ b/docs/adc-calibration.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomho\Development\Personal\food_thermometer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00581872-15E7-40D5-92D3-1759514EC87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC1B443-8EEC-4A16-9CC9-0DA51D3D0429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-110" windowWidth="37670" windowHeight="21820" activeTab="2" xr2:uid="{261724B8-50C6-4A72-A48F-8EC9FD2590B4}"/>
+    <workbookView xWindow="-16365" yWindow="3195" windowWidth="16530" windowHeight="28530" activeTab="3" xr2:uid="{261724B8-50C6-4A72-A48F-8EC9FD2590B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="espcal vs lut" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="15">
   <si>
     <t>Resistance:</t>
   </si>
@@ -59,6 +59,30 @@
   </si>
   <si>
     <t>Factor</t>
+  </si>
+  <si>
+    <t>~room</t>
+  </si>
+  <si>
+    <t>Raw</t>
+  </si>
+  <si>
+    <t>Esp-Cal</t>
+  </si>
+  <si>
+    <t>Lut-Esp-Cal</t>
+  </si>
+  <si>
+    <t>ice-water</t>
+  </si>
+  <si>
+    <t>hot tap</t>
+  </si>
+  <si>
+    <t>hot-tap-cooler</t>
+  </si>
+  <si>
+    <t>just-boiled (80)</t>
   </si>
 </sst>
 </file>
@@ -25981,6 +26005,1125 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'espcal vs lut'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lut-Esp-Cal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'espcal vs lut'!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1530</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2264</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2769</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2903</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3102</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'espcal vs lut'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2570</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2750</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3090</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-490E-4A84-9C4E-E54DBB0C1064}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="146355184"/>
+        <c:axId val="146374736"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="146355184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="146374736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="146374736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="146355184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'espcal vs lut'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Esp-Cal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'espcal vs lut'!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1392</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2631</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2807</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3135</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'espcal vs lut'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2570</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2750</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3090</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CA5E-48B7-96D3-963C95EC62A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1797716240"/>
+        <c:axId val="1788611680"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1797716240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1788611680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1788611680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1797716240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'espcal vs lut'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Raw</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'espcal vs lut'!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1522</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2383</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3071</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3362</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4057</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'espcal vs lut'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2570</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2750</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3090</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3996-46F5-AAFC-B1F74E8E27D0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1790101792"/>
+        <c:axId val="1790105120"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1790101792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1790105120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1790105120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1790101792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -26062,6 +27205,126 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -27649,6 +28912,1554 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -27764,6 +30575,119 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>144462</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>1587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F68B28E-8148-4467-B677-CA24A79EAED8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>36512</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EAA2F1C-E02D-459C-979F-CC214BA8A8F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>96837</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>131762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A5C645E-5739-4E53-B46D-CDC1F93A2071}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -65384,7 +68308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E0E8B01-7441-4EC2-AE89-8544F8391FD8}">
   <dimension ref="B1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1:I5"/>
     </sheetView>
   </sheetViews>
@@ -65922,4 +68846,165 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A476E6-817F-4E40-A05C-9E414CB0C06B}">
+  <dimension ref="A1:M61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>1360</v>
+      </c>
+      <c r="C2">
+        <v>1522</v>
+      </c>
+      <c r="D2">
+        <v>1392</v>
+      </c>
+      <c r="E2">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>2040</v>
+      </c>
+      <c r="C3">
+        <v>2383</v>
+      </c>
+      <c r="D3">
+        <v>2098</v>
+      </c>
+      <c r="E3">
+        <v>2264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>2570</v>
+      </c>
+      <c r="C4">
+        <v>3071</v>
+      </c>
+      <c r="D4">
+        <v>2631</v>
+      </c>
+      <c r="E4">
+        <v>2769</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>2750</v>
+      </c>
+      <c r="C5">
+        <v>3362</v>
+      </c>
+      <c r="D5">
+        <v>2807</v>
+      </c>
+      <c r="E5">
+        <v>2903</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>3090</v>
+      </c>
+      <c r="C6">
+        <v>4057</v>
+      </c>
+      <c r="D6">
+        <v>3135</v>
+      </c>
+      <c r="E6">
+        <v>3102</v>
+      </c>
+    </row>
+    <row r="40" spans="11:12" x14ac:dyDescent="0.35">
+      <c r="K40">
+        <v>79.3</v>
+      </c>
+      <c r="L40">
+        <v>79.7</v>
+      </c>
+    </row>
+    <row r="50" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="K50">
+        <v>82.3</v>
+      </c>
+      <c r="L50">
+        <v>81.7</v>
+      </c>
+      <c r="M50">
+        <f>L39/K50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="K60">
+        <v>24.6</v>
+      </c>
+      <c r="M60">
+        <f>L29/K60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="K61">
+        <v>84</v>
+      </c>
+      <c r="M61">
+        <f>L30/K61</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>